<commit_message>
Update project end milestone to 6 months from project start
Co-authored-by: esmaiel <esmaiel@gmail.com>
</commit_message>
<xml_diff>
--- a/urban_township_schedule.xlsx
+++ b/urban_township_schedule.xlsx
@@ -1620,14 +1620,14 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>پایان پروژه (۴ ماه)</t>
+          <t>پایان پروژه (۶ ماه)</t>
         </is>
       </c>
       <c r="C30" t="n">
         <v>1</v>
       </c>
       <c r="D30">
-        <f>NETWORKDAYS.INTL(Settings!$B$2, EDATE(Settings!$B$2, 4), Settings!$B$3, Holidays!$A$2:$A$1000) - C30</f>
+        <f>NETWORKDAYS.INTL(Settings!$B$2, EDATE(Settings!$B$2, 6), Settings!$B$3, Holidays!$A$2:$A$1000) - C30</f>
         <v/>
       </c>
       <c r="E30" s="1">
@@ -1640,7 +1640,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>نشانگر پایان ۴ ماهه</t>
+          <t>نشانگر پایان ۶ ماهه</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">

</xml_diff>